<commit_message>
make new copy of db
</commit_message>
<xml_diff>
--- a/Financial-1402-1 - Copy.xlsx
+++ b/Financial-1402-1 - Copy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\parham\guilan-univercity homeWork\Term 1402 - 1\financial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\parham\Programing\BootStrap Ex\python\financial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D07C37D-68BA-48DA-96D6-E2E53262D044}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7772819-5090-4958-9987-F73FA43936CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="save" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+  <si>
+    <t>id</t>
+  </si>
   <si>
     <t>month_id</t>
   </si>
@@ -40,10 +43,19 @@
     <t>sum</t>
   </si>
   <si>
+    <t>date</t>
+  </si>
+  <si>
     <t>save_id</t>
   </si>
   <si>
     <t>desc</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>time</t>
   </si>
   <si>
     <t>cost_id</t>
@@ -53,13 +65,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -70,7 +87,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -78,12 +95,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,29 +421,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -417,79 +458,97 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D507401F-E354-4CB1-B011-D560AD241DCB}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58682537-8DDF-49E4-8ABB-F5F0D9602E40}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC1E0A6-D72C-49D1-8919-4BE5B3BFB558}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add id field for log table
</commit_message>
<xml_diff>
--- a/Financial-1402-1 - Copy.xlsx
+++ b/Financial-1402-1 - Copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\parham\Programing\BootStrap Ex\python\financial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7772819-5090-4958-9987-F73FA43936CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D223A4-79DC-4F4B-BB2A-B0F0C6F95E2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="save" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t>id</t>
   </si>
@@ -65,13 +65,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -87,7 +92,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -110,13 +115,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -423,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,25 +482,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -490,32 +514,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -526,25 +550,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add total sheet to database, add update_total_table method
</commit_message>
<xml_diff>
--- a/Financial-1402-1 - Copy.xlsx
+++ b/Financial-1402-1 - Copy.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\parham\Programing\BootStrap Ex\python\financial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D223A4-79DC-4F4B-BB2A-B0F0C6F95E2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675F7591-A529-427E-9A56-E5450EF028F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="save" sheetId="1" r:id="rId1"/>
     <sheet name="save_log" sheetId="2" r:id="rId2"/>
     <sheet name="cost" sheetId="3" r:id="rId3"/>
     <sheet name="cost_log" sheetId="4" r:id="rId4"/>
+    <sheet name="total" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -59,6 +60,15 @@
   </si>
   <si>
     <t>cost_id</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>cost</t>
   </si>
 </sst>
 </file>
@@ -514,7 +524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -578,4 +588,36 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AEBD4B2-6DB1-41D8-9C04-946E032553B2}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>